<commit_message>
Corrected formula insert in excel_writer, Updated Readme
</commit_message>
<xml_diff>
--- a/outputs/output_davidsonco.xlsx
+++ b/outputs/output_davidsonco.xlsx
@@ -543,14 +543,17 @@
           <t>3.254</t>
         </is>
       </c>
-      <c r="L2" t="n">
-        <v>757700</v>
-      </c>
-      <c r="M2" t="n">
-        <v>303080</v>
-      </c>
-      <c r="N2" t="n">
-        <v>9862.2232</v>
+      <c r="L2">
+        <f>G2+H2</f>
+        <v/>
+      </c>
+      <c r="M2">
+        <f>L2*(J2/100)</f>
+        <v/>
+      </c>
+      <c r="N2">
+        <f>M2*(K2/100)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update scraping logic, improve concurrency, and fix minor error handling issues
</commit_message>
<xml_diff>
--- a/outputs/output_davidsonco.xlsx
+++ b/outputs/output_davidsonco.xlsx
@@ -524,23 +524,29 @@
           <t>152.00</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>664400</v>
-      </c>
-      <c r="H2" t="n">
-        <v>93300</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>664,400.00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>93,300.00</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>40.0%</t>
+          <t>40%</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>3.254</t>
+          <t>3.25400</t>
         </is>
       </c>
       <c r="L2">
@@ -548,7 +554,7 @@
         <v/>
       </c>
       <c r="M2">
-        <f>L2*(J2/100)</f>
+        <f>L2*(J2)</f>
         <v/>
       </c>
       <c r="N2">

</xml_diff>

<commit_message>
Updated README and roadmap with detailed features, installation steps, and usage instructions
</commit_message>
<xml_diff>
--- a/outputs/output_davidsonco.xlsx
+++ b/outputs/output_davidsonco.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,45 +449,50 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>Locale</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>Parcel</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Improvement Value</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Land Value</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Personal Property Value</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Assessment Rate</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Tax Rate</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Total Value</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Assessed Value</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Tax</t>
         </is>
@@ -496,69 +501,50 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>101 Hart Ln</t>
+          <t>200 N Trig</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>101 HART LANE, LLC</t>
+          <t>200 N TRIGG LLC</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>101 HART LN</t>
+          <t>126C-E-24.00--0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>06012015200</t>
+          <t>200 TRIGG AVENUE NORTH</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2024</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>152.00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>664,400.00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>93,300.00</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>40%</t>
-        </is>
-      </c>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>3.25400</t>
-        </is>
-      </c>
-      <c r="L2">
-        <f>G2+H2</f>
-        <v/>
-      </c>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2">
-        <f>L2*(J2)</f>
+        <f>H2+I2</f>
         <v/>
       </c>
       <c r="N2">
         <f>M2*(K2/100)</f>
+        <v/>
+      </c>
+      <c r="O2">
+        <f>N2*(L2/100)</f>
         <v/>
       </c>
     </row>

</xml_diff>